<commit_message>
Subida inicio de p6
</commit_message>
<xml_diff>
--- a/Practica4/Ejercicio12.xlsx
+++ b/Practica4/Ejercicio12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Massimo\Desktop\UNLP\2do año\segundo\ISO\Practica4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FFB3B82-1621-4AB1-A936-E1AA0CDAE1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6589B580-98EC-4395-858F-C0B0FF93C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3ABE947F-58F9-4D8F-A7AA-FD556D1FF562}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,9 +1013,7 @@
       <c r="O7" s="2">
         <v>4</v>
       </c>
-      <c r="P7" s="2">
-        <v>4</v>
-      </c>
+      <c r="P7" s="2"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>

</xml_diff>

<commit_message>
Subida mas ejercicios hechos
</commit_message>
<xml_diff>
--- a/Practica4/Ejercicio12.xlsx
+++ b/Practica4/Ejercicio12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Massimo\Desktop\UNLP\2do año\segundo\ISO\Practica4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6589B580-98EC-4395-858F-C0B0FF93C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB0842-7AE0-4077-AB27-32CD0D8B8A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3ABE947F-58F9-4D8F-A7AA-FD556D1FF562}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Job</t>
   </si>
@@ -154,15 +154,6 @@
   </si>
   <si>
     <t>4&lt;</t>
-  </si>
-  <si>
-    <t>6&lt;</t>
-  </si>
-  <si>
-    <t>5&lt;</t>
-  </si>
-  <si>
-    <t>2&lt;</t>
   </si>
   <si>
     <t>TE</t>
@@ -586,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085467C6-F572-4219-BEAF-D716A7BE2F1F}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,16 +682,16 @@
         <v>22</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -752,8 +743,8 @@
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
@@ -785,37 +776,23 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="7">
-        <v>3</v>
-      </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7">
-        <v>4</v>
-      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="7">
-        <v>5</v>
-      </c>
-      <c r="W3" s="4">
-        <v>2</v>
-      </c>
-      <c r="X3" s="4">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
@@ -839,21 +816,13 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>2</v>
-      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="7">
-        <v>3</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
@@ -864,8 +833,8 @@
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
@@ -894,38 +863,22 @@
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
-      <c r="P5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>2</v>
-      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="7">
-        <v>2</v>
-      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-      <c r="W5" s="7">
-        <v>3</v>
-      </c>
-      <c r="X5" s="6">
-        <v>3</v>
-      </c>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="7">
-        <v>4</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
@@ -957,12 +910,8 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="7">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
@@ -970,8 +919,8 @@
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
@@ -986,34 +935,24 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
         <v>3</v>
       </c>
-      <c r="I7" s="2">
+      <c r="K7" s="7">
         <v>2</v>
       </c>
-      <c r="J7" s="2">
-        <v>4</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3</v>
-      </c>
-      <c r="L7" s="2">
-        <v>5</v>
-      </c>
-      <c r="M7" s="2">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>4</v>
-      </c>
-      <c r="O7" s="2">
-        <v>4</v>
-      </c>
-      <c r="P7" s="2"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
@@ -1026,8 +965,8 @@
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
@@ -1039,21 +978,11 @@
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4</v>
-      </c>
-      <c r="I8" s="7">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>4</v>
-      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1072,8 +1001,8 @@
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
@@ -1085,12 +1014,8 @@
       <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1112,8 +1037,8 @@
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
@@ -1125,9 +1050,7 @@
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
+      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1150,8 +1073,8 @@
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
@@ -1163,12 +1086,8 @@
       <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4</v>
-      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1190,8 +1109,8 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>

</xml_diff>

<commit_message>
Subida p4 en pdf y mas completa
</commit_message>
<xml_diff>
--- a/Practica4/Ejercicio12.xlsx
+++ b/Practica4/Ejercicio12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Massimo\Desktop\UNLP\2do año\segundo\ISO\Practica4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB0842-7AE0-4077-AB27-32CD0D8B8A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C50A349-D822-4D0D-871E-5247A2A21CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3ABE947F-58F9-4D8F-A7AA-FD556D1FF562}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Job</t>
   </si>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t>TPE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>5&lt;</t>
+  </si>
+  <si>
+    <t>2&lt;</t>
+  </si>
+  <si>
+    <t>6&lt;</t>
   </si>
 </sst>
 </file>
@@ -217,12 +235,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -252,15 +288,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +616,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,41 +748,41 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7">
+      <c r="G2" s="6">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6">
         <v>3</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
@@ -764,35 +802,49 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="7">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
+      <c r="I3" s="6">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6">
+        <v>3</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6">
+        <v>4</v>
+      </c>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6">
+        <v>5</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
@@ -808,33 +860,41 @@
         <v>4</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
@@ -852,33 +912,47 @@
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6">
+        <v>3</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
@@ -894,33 +968,37 @@
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
@@ -942,31 +1020,43 @@
       <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="2">
         <v>3</v>
       </c>
-      <c r="K7" s="7">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>3</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>4</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
@@ -978,31 +1068,39 @@
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
@@ -1011,34 +1109,38 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
@@ -1047,34 +1149,36 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
@@ -1083,34 +1187,38 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>

</xml_diff>